<commit_message>
April 12th Update - Results section draft #1
</commit_message>
<xml_diff>
--- a/Species_list_SR_detailed.xlsx
+++ b/Species_list_SR_detailed.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wynnekat/Seed-Rain-Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wynnekat/SR---New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53925A1B-9DF5-1041-9584-E7EC5B5869BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BA7C39-8333-2740-B2B3-E79213738DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="1680" windowWidth="18600" windowHeight="17320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="7100" yWindow="740" windowWidth="18600" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$G$1:$G$129</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1895,7 +1895,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6502,6 +6502,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="G1:G129" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>